<commit_message>
commit on develop. adding all files in
</commit_message>
<xml_diff>
--- a/data/labyrinthe.xlsx
+++ b/data/labyrinthe.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\02_oc\03_p3\02_project\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\02_oc\03_p3\02_project\P3\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{01F63BA5-CA1A-487B-826E-12552A5D35CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EADAC6AC-16A1-4B9B-9474-BB1D7709B5DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16650" yWindow="-15420" windowWidth="11055" windowHeight="9165" xr2:uid="{E4DBB735-3FCB-492F-8577-E7CB6FF5332F}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{E4DBB735-3FCB-492F-8577-E7CB6FF5332F}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -30,6 +30,17 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="2">
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>nb si</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -394,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E756F10B-B9A3-4446-8E49-989FB0575E26}">
-  <dimension ref="A1:O25"/>
+  <dimension ref="A1:Q25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -405,7 +416,7 @@
     <col min="1" max="15" width="2.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -422,144 +433,429 @@
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
     </row>
-    <row r="2" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
+      <c r="E2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" t="s">
+        <v>0</v>
+      </c>
       <c r="J2" s="1"/>
-      <c r="L2" s="3"/>
+      <c r="K2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>0</v>
+      </c>
       <c r="O2" s="1"/>
-    </row>
-    <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>0</v>
+      </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
+      <c r="I3" t="s">
+        <v>0</v>
+      </c>
+      <c r="J3" t="s">
+        <v>0</v>
+      </c>
+      <c r="K3" t="s">
+        <v>0</v>
+      </c>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
-    </row>
-    <row r="4" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q3">
+        <f>COUNTIF(A1:O15,"x")</f>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
-      <c r="I4" s="3"/>
+      <c r="I4" s="3" t="s">
+        <v>0</v>
+      </c>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
-      <c r="L4" s="3"/>
+      <c r="L4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="M4" t="s">
+        <v>0</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>0</v>
+      </c>
       <c r="O4" s="1"/>
     </row>
-    <row r="5" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
+      <c r="B5" t="s">
+        <v>0</v>
+      </c>
       <c r="C5" s="1"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
+      <c r="D5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>0</v>
+      </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
-      <c r="L5" s="3"/>
+      <c r="L5" s="3" t="s">
+        <v>0</v>
+      </c>
       <c r="M5" s="1"/>
+      <c r="N5" s="3" t="s">
+        <v>0</v>
+      </c>
       <c r="O5" s="1"/>
     </row>
-    <row r="6" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
+      <c r="B6" t="s">
+        <v>0</v>
+      </c>
       <c r="C6" s="1"/>
+      <c r="D6" t="s">
+        <v>0</v>
+      </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
+      <c r="G6" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="J6" t="s">
+        <v>0</v>
+      </c>
       <c r="K6" s="1"/>
+      <c r="L6" s="3" t="s">
+        <v>0</v>
+      </c>
       <c r="M6" s="1"/>
+      <c r="N6" s="3" t="s">
+        <v>0</v>
+      </c>
       <c r="O6" s="1"/>
     </row>
-    <row r="7" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
+      <c r="B7" t="s">
+        <v>0</v>
+      </c>
       <c r="C7" s="1"/>
+      <c r="D7" t="s">
+        <v>0</v>
+      </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
+      <c r="J7" t="s">
+        <v>0</v>
+      </c>
+      <c r="K7" t="s">
+        <v>0</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>0</v>
+      </c>
       <c r="M7" s="1"/>
+      <c r="N7" s="3" t="s">
+        <v>0</v>
+      </c>
       <c r="O7" s="1"/>
     </row>
-    <row r="8" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="2"/>
+    <row r="8" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>0</v>
+      </c>
       <c r="C8" s="1"/>
+      <c r="D8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8" t="s">
+        <v>0</v>
+      </c>
+      <c r="F8" t="s">
+        <v>0</v>
+      </c>
+      <c r="G8" t="s">
+        <v>0</v>
+      </c>
+      <c r="H8" t="s">
+        <v>0</v>
+      </c>
+      <c r="I8" t="s">
+        <v>0</v>
+      </c>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
+      <c r="L8" s="3" t="s">
+        <v>0</v>
+      </c>
       <c r="M8" s="1"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="3"/>
-    </row>
-    <row r="9" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N8" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
+      <c r="B9" t="s">
+        <v>0</v>
+      </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
+      <c r="G9" t="s">
+        <v>0</v>
+      </c>
       <c r="H9" s="1"/>
+      <c r="I9" t="s">
+        <v>0</v>
+      </c>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
+      <c r="L9" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="M9" t="s">
+        <v>0</v>
+      </c>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
     </row>
-    <row r="10" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
+      <c r="B10" t="s">
+        <v>0</v>
+      </c>
       <c r="C10" s="1"/>
+      <c r="D10" t="s">
+        <v>0</v>
+      </c>
+      <c r="E10" t="s">
+        <v>0</v>
+      </c>
+      <c r="F10" t="s">
+        <v>0</v>
+      </c>
+      <c r="G10" t="s">
+        <v>0</v>
+      </c>
       <c r="H10" s="1"/>
+      <c r="I10" t="s">
+        <v>0</v>
+      </c>
+      <c r="J10" t="s">
+        <v>0</v>
+      </c>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
+      <c r="M10" t="s">
+        <v>0</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>0</v>
+      </c>
       <c r="O10" s="1"/>
     </row>
-    <row r="11" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
+      <c r="B11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" t="s">
+        <v>0</v>
+      </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
+      <c r="J11" t="s">
+        <v>0</v>
+      </c>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
     </row>
-    <row r="12" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
+      <c r="B12" t="s">
+        <v>0</v>
+      </c>
       <c r="C12" s="1"/>
+      <c r="D12" t="s">
+        <v>0</v>
+      </c>
       <c r="E12" s="1"/>
+      <c r="F12" t="s">
+        <v>0</v>
+      </c>
+      <c r="G12" t="s">
+        <v>0</v>
+      </c>
+      <c r="H12" t="s">
+        <v>0</v>
+      </c>
       <c r="I12" s="1"/>
+      <c r="J12" t="s">
+        <v>0</v>
+      </c>
+      <c r="K12" t="s">
+        <v>0</v>
+      </c>
       <c r="L12" s="1"/>
+      <c r="M12" t="s">
+        <v>0</v>
+      </c>
+      <c r="N12" s="3" t="s">
+        <v>0</v>
+      </c>
       <c r="O12" s="1"/>
     </row>
-    <row r="13" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
+      <c r="B13" t="s">
+        <v>0</v>
+      </c>
       <c r="C13" s="1"/>
+      <c r="D13" t="s">
+        <v>0</v>
+      </c>
       <c r="E13" s="1"/>
+      <c r="F13" t="s">
+        <v>0</v>
+      </c>
       <c r="G13" s="1"/>
+      <c r="H13" t="s">
+        <v>0</v>
+      </c>
       <c r="I13" s="1"/>
+      <c r="J13" t="s">
+        <v>0</v>
+      </c>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
+      <c r="M13" t="s">
+        <v>0</v>
+      </c>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
     </row>
-    <row r="14" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
+      <c r="B14" t="s">
+        <v>0</v>
+      </c>
       <c r="C14" s="1"/>
+      <c r="D14" t="s">
+        <v>0</v>
+      </c>
+      <c r="E14" t="s">
+        <v>0</v>
+      </c>
+      <c r="F14" t="s">
+        <v>0</v>
+      </c>
       <c r="G14" s="1"/>
+      <c r="H14" t="s">
+        <v>0</v>
+      </c>
       <c r="I14" s="1"/>
+      <c r="J14" t="s">
+        <v>0</v>
+      </c>
+      <c r="K14" t="s">
+        <v>0</v>
+      </c>
+      <c r="L14" t="s">
+        <v>0</v>
+      </c>
+      <c r="M14" t="s">
+        <v>0</v>
+      </c>
+      <c r="N14" t="s">
+        <v>0</v>
+      </c>
       <c r="O14" s="1"/>
     </row>
-    <row r="15" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -576,7 +872,7 @@
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
     </row>
-    <row r="16" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="17" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="18" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="19" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
commit on develop. class Cell, Object, MacGyver are clean
</commit_message>
<xml_diff>
--- a/data/labyrinthe.xlsx
+++ b/data/labyrinthe.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\02_oc\03_p3\02_project\P3\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EADAC6AC-16A1-4B9B-9474-BB1D7709B5DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B7573B7-031B-4EB1-866F-275D6686020E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{E4DBB735-3FCB-492F-8577-E7CB6FF5332F}"/>
+    <workbookView xWindow="10290" yWindow="-16050" windowWidth="16920" windowHeight="13575" xr2:uid="{E4DBB735-3FCB-492F-8577-E7CB6FF5332F}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -33,12 +33,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="1">
   <si>
     <t>x</t>
-  </si>
-  <si>
-    <t>nb si</t>
   </si>
 </sst>
 </file>
@@ -54,7 +51,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -73,8 +70,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -82,15 +85,38 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -405,18 +431,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E756F10B-B9A3-4446-8E49-989FB0575E26}">
-  <dimension ref="A1:Q25"/>
+  <dimension ref="A1:Q33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R14" sqref="R14"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="15" width="2.77734375" customWidth="1"/>
+    <col min="16" max="16" width="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="2.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -433,7 +461,7 @@
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
     </row>
-    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" t="s">
         <v>0</v>
@@ -469,11 +497,8 @@
         <v>0</v>
       </c>
       <c r="O2" s="1"/>
-      <c r="Q2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" t="s">
         <v>0</v>
@@ -503,12 +528,8 @@
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
-      <c r="Q3">
-        <f>COUNTIF(A1:O15,"x")</f>
-        <v>97</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" t="s">
         <v>0</v>
@@ -535,7 +556,7 @@
       </c>
       <c r="O4" s="1"/>
     </row>
-    <row r="5" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" t="s">
         <v>0</v>
@@ -566,7 +587,7 @@
       </c>
       <c r="O5" s="1"/>
     </row>
-    <row r="6" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" t="s">
         <v>0</v>
@@ -599,7 +620,7 @@
       </c>
       <c r="O6" s="1"/>
     </row>
-    <row r="7" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" t="s">
         <v>0</v>
@@ -628,7 +649,7 @@
       </c>
       <c r="O7" s="1"/>
     </row>
-    <row r="8" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>0</v>
       </c>
@@ -667,7 +688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" t="s">
         <v>0</v>
@@ -694,7 +715,7 @@
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
     </row>
-    <row r="10" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" t="s">
         <v>0</v>
@@ -729,7 +750,7 @@
       </c>
       <c r="O10" s="1"/>
     </row>
-    <row r="11" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" t="s">
         <v>0</v>
@@ -754,7 +775,7 @@
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
     </row>
-    <row r="12" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" t="s">
         <v>0</v>
@@ -789,7 +810,7 @@
       </c>
       <c r="O12" s="1"/>
     </row>
-    <row r="13" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" t="s">
         <v>0</v>
@@ -818,7 +839,7 @@
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
     </row>
-    <row r="14" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" t="s">
         <v>0</v>
@@ -855,7 +876,7 @@
       </c>
       <c r="O14" s="1"/>
     </row>
-    <row r="15" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -872,16 +893,565 @@
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
     </row>
-    <row r="16" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="17" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="18" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="19" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="20" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="21" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="22" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="23" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="24" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="25" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="18" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="9">
+        <v>0</v>
+      </c>
+      <c r="D18" s="9">
+        <v>1</v>
+      </c>
+      <c r="E18" s="9">
+        <v>2</v>
+      </c>
+      <c r="F18" s="9">
+        <v>3</v>
+      </c>
+      <c r="G18" s="9">
+        <v>4</v>
+      </c>
+      <c r="H18" s="9">
+        <v>5</v>
+      </c>
+      <c r="I18" s="9">
+        <v>6</v>
+      </c>
+      <c r="J18" s="9">
+        <v>7</v>
+      </c>
+      <c r="K18" s="9">
+        <v>8</v>
+      </c>
+      <c r="L18" s="9">
+        <v>9</v>
+      </c>
+      <c r="M18" s="9">
+        <v>10</v>
+      </c>
+      <c r="N18" s="9">
+        <v>11</v>
+      </c>
+      <c r="O18" s="9">
+        <v>12</v>
+      </c>
+      <c r="P18" s="9">
+        <v>13</v>
+      </c>
+      <c r="Q18" s="9">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="4"/>
+      <c r="B19" s="7">
+        <v>0</v>
+      </c>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="5"/>
+      <c r="O19" s="5"/>
+      <c r="P19" s="5"/>
+      <c r="Q19" s="5"/>
+    </row>
+    <row r="20" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="4"/>
+      <c r="B20" s="7">
+        <v>1</v>
+      </c>
+      <c r="C20" s="5"/>
+      <c r="D20" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="J20" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="K20" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L20" s="5"/>
+      <c r="M20" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="N20" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="O20" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="P20" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="5"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A21" s="4"/>
+      <c r="B21" s="7">
+        <v>2</v>
+      </c>
+      <c r="C21" s="5"/>
+      <c r="D21" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L21" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="M21" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="N21" s="5"/>
+      <c r="O21" s="5"/>
+      <c r="P21" s="5"/>
+      <c r="Q21" s="5"/>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A22" s="4"/>
+      <c r="B22" s="7">
+        <v>3</v>
+      </c>
+      <c r="C22" s="5"/>
+      <c r="D22" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="O22" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="P22" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="5"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A23" s="4"/>
+      <c r="B23" s="7">
+        <v>4</v>
+      </c>
+      <c r="C23" s="5"/>
+      <c r="D23" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E23" s="5"/>
+      <c r="F23" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="H23" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="I23" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="O23" s="5"/>
+      <c r="P23" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="5"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A24" s="4"/>
+      <c r="B24" s="7">
+        <v>5</v>
+      </c>
+      <c r="C24" s="5"/>
+      <c r="D24" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E24" s="5"/>
+      <c r="F24" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="J24" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="K24" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="L24" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="M24" s="5"/>
+      <c r="N24" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="O24" s="5"/>
+      <c r="P24" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="5"/>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A25" s="4"/>
+      <c r="B25" s="7">
+        <v>6</v>
+      </c>
+      <c r="C25" s="5"/>
+      <c r="D25" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E25" s="5"/>
+      <c r="F25" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="5"/>
+      <c r="L25" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="M25" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="N25" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="O25" s="5"/>
+      <c r="P25" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q25" s="5"/>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A26" s="4"/>
+      <c r="B26" s="7">
+        <v>7</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E26" s="5"/>
+      <c r="F26" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="H26" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="I26" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="J26" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="K26" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L26" s="5"/>
+      <c r="M26" s="5"/>
+      <c r="N26" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="O26" s="5"/>
+      <c r="P26" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A27" s="4"/>
+      <c r="B27" s="7">
+        <v>8</v>
+      </c>
+      <c r="C27" s="5"/>
+      <c r="D27" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="J27" s="5"/>
+      <c r="K27" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L27" s="5"/>
+      <c r="M27" s="5"/>
+      <c r="N27" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="O27" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="P27" s="5"/>
+      <c r="Q27" s="5"/>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A28" s="4"/>
+      <c r="B28" s="7">
+        <v>9</v>
+      </c>
+      <c r="C28" s="5"/>
+      <c r="D28" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E28" s="5"/>
+      <c r="F28" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="H28" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="I28" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="J28" s="5"/>
+      <c r="K28" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L28" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="M28" s="5"/>
+      <c r="N28" s="5"/>
+      <c r="O28" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="P28" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="5"/>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A29" s="4"/>
+      <c r="B29" s="7">
+        <v>10</v>
+      </c>
+      <c r="C29" s="5"/>
+      <c r="D29" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="5"/>
+      <c r="L29" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="M29" s="5"/>
+      <c r="N29" s="5"/>
+      <c r="O29" s="5"/>
+      <c r="P29" s="5"/>
+      <c r="Q29" s="5"/>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A30" s="4"/>
+      <c r="B30" s="7">
+        <v>11</v>
+      </c>
+      <c r="C30" s="5"/>
+      <c r="D30" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E30" s="5"/>
+      <c r="F30" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G30" s="5"/>
+      <c r="H30" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="I30" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="J30" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="K30" s="5"/>
+      <c r="L30" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="M30" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="N30" s="5"/>
+      <c r="O30" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="P30" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q30" s="5"/>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A31" s="4"/>
+      <c r="B31" s="7">
+        <v>12</v>
+      </c>
+      <c r="C31" s="5"/>
+      <c r="D31" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E31" s="5"/>
+      <c r="F31" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G31" s="5"/>
+      <c r="H31" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="I31" s="5"/>
+      <c r="J31" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="K31" s="5"/>
+      <c r="L31" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="M31" s="5"/>
+      <c r="N31" s="5"/>
+      <c r="O31" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="P31" s="5"/>
+      <c r="Q31" s="5"/>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A32" s="4"/>
+      <c r="B32" s="7">
+        <v>13</v>
+      </c>
+      <c r="C32" s="5"/>
+      <c r="D32" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E32" s="5"/>
+      <c r="F32" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="H32" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="I32" s="5"/>
+      <c r="J32" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="K32" s="5"/>
+      <c r="L32" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="M32" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="N32" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="O32" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="P32" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q32" s="5"/>
+    </row>
+    <row r="33" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B33" s="7">
+        <v>14</v>
+      </c>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="5"/>
+      <c r="J33" s="5"/>
+      <c r="K33" s="5"/>
+      <c r="L33" s="5"/>
+      <c r="M33" s="5"/>
+      <c r="N33" s="5"/>
+      <c r="O33" s="5"/>
+      <c r="P33" s="5"/>
+      <c r="Q33" s="5"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>